<commit_message>
end of the trainig part
</commit_message>
<xml_diff>
--- a/Training_update.xlsx
+++ b/Training_update.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="45">
   <si>
     <t xml:space="preserve"> S. No.</t>
   </si>
@@ -31,12 +31,6 @@
     <t xml:space="preserve">Sub-topic</t>
   </si>
   <si>
-    <t xml:space="preserve">Start date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">End date</t>
-  </si>
-  <si>
     <t xml:space="preserve">Status</t>
   </si>
   <si>
@@ -49,18 +43,27 @@
     <t xml:space="preserve">IPV4 TCP Sockets</t>
   </si>
   <si>
+    <t xml:space="preserve">Done</t>
+  </si>
+  <si>
     <t xml:space="preserve">IPV4 UDP sockets</t>
   </si>
   <si>
     <t xml:space="preserve">IPV6 TCP &amp; UDP Socket</t>
   </si>
   <si>
+    <t xml:space="preserve">done with the TCP ipv6 part UDP ipv6 is remaining</t>
+  </si>
+  <si>
     <t xml:space="preserve">Multi threading</t>
   </si>
   <si>
     <t xml:space="preserve">Pthread creation</t>
   </si>
   <si>
+    <t xml:space="preserve">done with the theory part</t>
+  </si>
+  <si>
     <t xml:space="preserve">wait objects</t>
   </si>
   <si>
@@ -79,6 +82,9 @@
     <t xml:space="preserve">STL</t>
   </si>
   <si>
+    <t xml:space="preserve">work on std::arrays , std::vector </t>
+  </si>
+  <si>
     <t xml:space="preserve">maps</t>
   </si>
   <si>
@@ -112,27 +118,53 @@
     <t xml:space="preserve">Android build server</t>
   </si>
   <si>
+    <t xml:space="preserve">Tried the connection with the vcu using android debug build commands</t>
+  </si>
+  <si>
     <t xml:space="preserve">Copying binaries to VCU</t>
   </si>
   <si>
     <t xml:space="preserve">Executing binaries.</t>
   </si>
   <si>
+    <t xml:space="preserve"> Seen the testing part of the hardware once.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Git</t>
   </si>
   <si>
     <t xml:space="preserve">commands of git</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LUNIX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">commands of lunix </t>
+  </si>
+  <si>
+    <t xml:space="preserve">G_Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit Testing in cpp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Library Creation in cpp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adb commands</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -168,8 +200,21 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -232,49 +277,45 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="9" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="9" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="9" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="9" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -355,45 +396,37 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1048576"/>
+  <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="21.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="22.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="26.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="16.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="22.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="65.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="2" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="26.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="22.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="65.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="6" style="1" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="21.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -401,14 +434,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="9"/>
+        <v>6</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="21.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="n">
@@ -416,11 +449,11 @@
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="9"/>
+        <v>8</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="21.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="n">
@@ -428,14 +461,17 @@
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="9"/>
     </row>
     <row r="5" customFormat="false" ht="21.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="n">
+      <c r="A5" s="9" t="n">
         <v>2</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -445,197 +481,256 @@
         <v>12</v>
       </c>
       <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9"/>
+      <c r="E5" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="21.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="9"/>
+        <v>14</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="21.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="6"/>
       <c r="C7" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="9"/>
+        <v>15</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="21.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="6"/>
       <c r="C8" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="9"/>
+        <v>16</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="21.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="9"/>
+        <v>17</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="21.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="n">
+      <c r="A10" s="9" t="n">
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="9"/>
+        <v>19</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="21.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="6"/>
       <c r="C11" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="9"/>
+        <v>21</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="6"/>
       <c r="C12" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="9"/>
+        <v>22</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="21.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="6"/>
       <c r="C13" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="21.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10"/>
+      <c r="A14" s="9"/>
       <c r="B14" s="6"/>
       <c r="C14" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="9"/>
+        <v>24</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="21.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="10"/>
+      <c r="A15" s="9"/>
       <c r="B15" s="6"/>
       <c r="C15" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="9"/>
+        <v>25</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="21.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10" t="n">
+      <c r="A16" s="9" t="n">
         <v>5</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="9"/>
     </row>
     <row r="17" customFormat="false" ht="21.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10"/>
+      <c r="A17" s="9"/>
       <c r="B17" s="6"/>
       <c r="C17" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="9"/>
     </row>
     <row r="18" customFormat="false" ht="21.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="10"/>
+      <c r="A18" s="9"/>
       <c r="B18" s="6"/>
       <c r="C18" s="7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="9"/>
     </row>
     <row r="19" customFormat="false" ht="21.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="10" t="n">
+      <c r="A19" s="9" t="n">
         <v>6</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="9"/>
+      <c r="E19" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="21.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="10"/>
+      <c r="A20" s="9"/>
       <c r="B20" s="6"/>
       <c r="C20" s="7" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="9"/>
     </row>
     <row r="21" customFormat="false" ht="21.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="10"/>
+      <c r="A21" s="9"/>
       <c r="B21" s="6"/>
       <c r="C21" s="7" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="9"/>
-    </row>
-    <row r="22" customFormat="false" ht="21.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E21" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="19.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="B22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="19.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="19.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="20.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="1048576" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="10">

</xml_diff>